<commit_message>
update 21 Agustus 2021
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KARANGPLOSO" sheetId="1" r:id="rId1"/>
     <sheet name="PENDEM" sheetId="2" r:id="rId2"/>
     <sheet name="GPA" sheetId="3" r:id="rId3"/>
     <sheet name="BABAAN" sheetId="4" r:id="rId4"/>
+    <sheet name="SUDAH MEMILIH" sheetId="5" r:id="rId5"/>
+    <sheet name="BELUM MEMILIH" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
   <si>
     <t>No.</t>
   </si>
@@ -39,6 +41,12 @@
   </si>
   <si>
     <t>Jumlah Suara</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -485,7 +493,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,4 +566,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="36.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="36.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>